<commit_message>
updated document based on feedback
</commit_message>
<xml_diff>
--- a/fsidemo/Dashbords and Reports for FSI.xlsx
+++ b/fsidemo/Dashbords and Reports for FSI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chouhan_rna\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B4FBA5E-9E6F-4C08-8FE8-02AEA684955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116849A6-F3D7-45D3-A0F5-04391961B5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{38D09F39-0E76-4E9B-96E9-E5DB56FB0FCE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="226">
   <si>
     <t>Dashboard</t>
   </si>
@@ -615,9 +615,6 @@
     <t>Revenue</t>
   </si>
   <si>
-    <t>Woodgrove Portfolio</t>
-  </si>
-  <si>
     <t>Asset Management chart</t>
   </si>
   <si>
@@ -706,6 +703,15 @@
   </si>
   <si>
     <t>FinalImage, 14042021</t>
+  </si>
+  <si>
+    <t>Woodgrove Portfolio Dec</t>
+  </si>
+  <si>
+    <t>Woodgrove Portfolio Jun</t>
+  </si>
+  <si>
+    <t>Woodgrove Portfolio mar</t>
   </si>
 </sst>
 </file>
@@ -1169,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2170F742-0D62-435A-B783-987EE966FD79}">
   <dimension ref="A1:E256"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E243" sqref="E243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2207,7 +2213,7 @@
         <v>95</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>96</v>
@@ -2274,7 +2280,7 @@
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="8"/>
       <c r="B81" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>96</v>
@@ -2354,7 +2360,7 @@
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="8"/>
       <c r="B87" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>96</v>
@@ -2434,7 +2440,7 @@
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="8"/>
       <c r="B93" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>96</v>
@@ -2517,10 +2523,10 @@
         <v>121</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>38</v>
@@ -3592,7 +3598,7 @@
         <v>185</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
@@ -3607,7 +3613,7 @@
         <v>187</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
@@ -3622,7 +3628,7 @@
         <v>180</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
@@ -3637,7 +3643,7 @@
         <v>180</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
@@ -3652,7 +3658,7 @@
         <v>184</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
@@ -3667,7 +3673,7 @@
         <v>180</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
@@ -3682,7 +3688,7 @@
         <v>187</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
@@ -3697,7 +3703,7 @@
         <v>187</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
@@ -3712,7 +3718,7 @@
         <v>184</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
@@ -3727,7 +3733,7 @@
         <v>184</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
@@ -3742,7 +3748,7 @@
         <v>184</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
@@ -3757,7 +3763,7 @@
         <v>184</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
@@ -3766,13 +3772,13 @@
         <v>113</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D186" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
@@ -3781,18 +3787,18 @@
         <v>113</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D187" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>6</v>
@@ -3861,7 +3867,7 @@
         <v>179</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>188</v>
@@ -3876,7 +3882,7 @@
         <v>179</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>189</v>
@@ -3939,7 +3945,7 @@
         <v>185</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
@@ -3951,10 +3957,10 @@
         <v>179</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
@@ -3969,7 +3975,7 @@
         <v>180</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
@@ -3984,7 +3990,7 @@
         <v>180</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
@@ -3999,7 +4005,7 @@
         <v>152</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
@@ -4014,7 +4020,7 @@
         <v>180</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
@@ -4026,10 +4032,10 @@
         <v>179</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
@@ -4041,10 +4047,10 @@
         <v>179</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
@@ -4059,7 +4065,7 @@
         <v>152</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
@@ -4074,7 +4080,7 @@
         <v>152</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
@@ -4089,7 +4095,7 @@
         <v>152</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
@@ -4104,7 +4110,7 @@
         <v>152</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
@@ -4116,10 +4122,10 @@
         <v>32</v>
       </c>
       <c r="D209" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E209" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
@@ -4134,12 +4140,12 @@
         <v>48</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>6</v>
@@ -4208,7 +4214,7 @@
         <v>179</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>188</v>
@@ -4223,7 +4229,7 @@
         <v>179</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>189</v>
@@ -4286,7 +4292,7 @@
         <v>185</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
@@ -4298,10 +4304,10 @@
         <v>179</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
@@ -4316,7 +4322,7 @@
         <v>180</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
@@ -4331,7 +4337,7 @@
         <v>180</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
@@ -4346,7 +4352,7 @@
         <v>152</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
@@ -4361,7 +4367,7 @@
         <v>180</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
@@ -4373,10 +4379,10 @@
         <v>179</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
@@ -4388,10 +4394,10 @@
         <v>179</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
@@ -4406,7 +4412,7 @@
         <v>152</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
@@ -4421,7 +4427,7 @@
         <v>152</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
@@ -4436,7 +4442,7 @@
         <v>152</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
@@ -4451,7 +4457,7 @@
         <v>152</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
@@ -4463,10 +4469,10 @@
         <v>32</v>
       </c>
       <c r="D232" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E232" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
@@ -4481,12 +4487,12 @@
         <v>48</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>6</v>
@@ -4555,7 +4561,7 @@
         <v>179</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E238" s="1" t="s">
         <v>188</v>
@@ -4570,7 +4576,7 @@
         <v>179</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E239" s="1" t="s">
         <v>189</v>
@@ -4633,7 +4639,7 @@
         <v>185</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
@@ -4645,10 +4651,10 @@
         <v>179</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
@@ -4663,7 +4669,7 @@
         <v>180</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
@@ -4678,7 +4684,7 @@
         <v>180</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
@@ -4693,7 +4699,7 @@
         <v>184</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
@@ -4708,7 +4714,7 @@
         <v>180</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
@@ -4720,10 +4726,10 @@
         <v>179</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
@@ -4735,10 +4741,10 @@
         <v>179</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
@@ -4753,7 +4759,7 @@
         <v>184</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
@@ -4768,7 +4774,7 @@
         <v>184</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.3">
@@ -4783,7 +4789,7 @@
         <v>184</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
@@ -4798,7 +4804,7 @@
         <v>184</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
@@ -4810,10 +4816,10 @@
         <v>32</v>
       </c>
       <c r="D255" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
@@ -4828,7 +4834,7 @@
         <v>48</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>